<commit_message>
add tkinter and update code for function
</commit_message>
<xml_diff>
--- a/Associate.xlsx
+++ b/Associate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4919" uniqueCount="292">
   <si>
     <t>ស្រី</t>
   </si>
@@ -688,51 +688,27 @@
     </r>
   </si>
   <si>
-    <t>٢ មករា ២០០១</t>
-  </si>
-  <si>
     <t>2 January 2001</t>
   </si>
   <si>
-    <t>١٠ ឧសភា ២០០៣</t>
-  </si>
-  <si>
     <t>10 May 2003</t>
   </si>
   <si>
-    <t>٢١ កុម្ភៈ ២០០៣</t>
-  </si>
-  <si>
     <t>21 February 2003</t>
   </si>
   <si>
-    <t>١٨ តុលា ២០០២</t>
-  </si>
-  <si>
     <t>18 October 2002</t>
   </si>
   <si>
-    <t>١٠ មករា ១៩៩៨</t>
-  </si>
-  <si>
     <t>10 January 1998</t>
   </si>
   <si>
-    <t>١٤ ឧសភា ២០០៣</t>
-  </si>
-  <si>
     <t>14 May 2003</t>
   </si>
   <si>
-    <t>٢٤ តុលា ២០០២</t>
-  </si>
-  <si>
     <t>24 October 2002</t>
   </si>
   <si>
-    <t>١٠ មេសា ២០០៣</t>
-  </si>
-  <si>
     <t>10 April 2003</t>
   </si>
   <si>
@@ -740,6 +716,210 @@
   </si>
   <si>
     <t>Exam day</t>
+  </si>
+  <si>
+    <t>Nov-26-24</t>
+  </si>
+  <si>
+    <t>Nov-26-25</t>
+  </si>
+  <si>
+    <t>Nov-26-26</t>
+  </si>
+  <si>
+    <t>Nov-26-27</t>
+  </si>
+  <si>
+    <t>Nov-26-28</t>
+  </si>
+  <si>
+    <t>Nov-26-29</t>
+  </si>
+  <si>
+    <t>Nov-26-30</t>
+  </si>
+  <si>
+    <t>Nov-26-31</t>
+  </si>
+  <si>
+    <t>Nov-26-32</t>
+  </si>
+  <si>
+    <t>Nov-26-33</t>
+  </si>
+  <si>
+    <t>Nov-26-34</t>
+  </si>
+  <si>
+    <t>Nov-26-35</t>
+  </si>
+  <si>
+    <t>Nov-26-36</t>
+  </si>
+  <si>
+    <t>Nov-26-37</t>
+  </si>
+  <si>
+    <t>Nov-26-38</t>
+  </si>
+  <si>
+    <t>Nov-26-39</t>
+  </si>
+  <si>
+    <t>Nov-26-40</t>
+  </si>
+  <si>
+    <t>Nov-26-41</t>
+  </si>
+  <si>
+    <t>Nov-26-42</t>
+  </si>
+  <si>
+    <t>Nov-26-43</t>
+  </si>
+  <si>
+    <t>Nov-26-44</t>
+  </si>
+  <si>
+    <t>Nov-26-45</t>
+  </si>
+  <si>
+    <t>Nov-26-46</t>
+  </si>
+  <si>
+    <t>Nov-26-47</t>
+  </si>
+  <si>
+    <t>Nov-26-48</t>
+  </si>
+  <si>
+    <t>Nov-26-49</t>
+  </si>
+  <si>
+    <t>Nov-26-50</t>
+  </si>
+  <si>
+    <t>Nov-26-51</t>
+  </si>
+  <si>
+    <t>Nov-26-52</t>
+  </si>
+  <si>
+    <t>Nov-26-53</t>
+  </si>
+  <si>
+    <t>Nov-26-54</t>
+  </si>
+  <si>
+    <t>Nov-26-55</t>
+  </si>
+  <si>
+    <t>Nov-26-56</t>
+  </si>
+  <si>
+    <t>Nov-26-57</t>
+  </si>
+  <si>
+    <t>Nov-26-58</t>
+  </si>
+  <si>
+    <t>Nov-26-59</t>
+  </si>
+  <si>
+    <t>Nov-26-60</t>
+  </si>
+  <si>
+    <t>Nov-26-61</t>
+  </si>
+  <si>
+    <t>Nov-26-62</t>
+  </si>
+  <si>
+    <t>Nov-26-63</t>
+  </si>
+  <si>
+    <t>Nov-26-64</t>
+  </si>
+  <si>
+    <t>Nov-26-65</t>
+  </si>
+  <si>
+    <t>Nov-26-66</t>
+  </si>
+  <si>
+    <t>Nov-26-67</t>
+  </si>
+  <si>
+    <t>Nov-26-68</t>
+  </si>
+  <si>
+    <t>Nov-26-69</t>
+  </si>
+  <si>
+    <t>٢٨ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>٢٩ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១២ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១៤ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២០ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២៣ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២៦ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៣១ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១០ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៥ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៣ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៨٠ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៨ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៤ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>៣០ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២២ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២១ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១៦ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>១៩ កញ្ញា ២០០៣</t>
+  </si>
+  <si>
+    <t>២៧ កញ្ញា ២០០៣</t>
   </si>
 </sst>
 </file>
@@ -1240,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1475,7 @@
         <v>213</v>
       </c>
       <c r="L1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1332,8 +1512,8 @@
       <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="24">
-        <v>45608</v>
+      <c r="L2" s="24" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1368,10 +1548,10 @@
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>230</v>
-      </c>
-      <c r="L3" s="24">
-        <v>45609</v>
+        <v>222</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,10 +1586,10 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>230</v>
-      </c>
-      <c r="L4" s="24">
-        <v>45610</v>
+        <v>222</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1444,10 +1624,10 @@
         <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>230</v>
-      </c>
-      <c r="L5" s="24">
-        <v>45611</v>
+        <v>222</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1482,10 +1662,10 @@
         <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L6" s="24">
-        <v>45612</v>
+        <v>222</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1520,10 +1700,10 @@
         <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>230</v>
-      </c>
-      <c r="L7" s="24">
-        <v>45613</v>
+        <v>222</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1558,10 +1738,10 @@
         <v>202</v>
       </c>
       <c r="K8" t="s">
+        <v>222</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>230</v>
-      </c>
-      <c r="L8" s="24">
-        <v>45614</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1596,10 +1776,10 @@
         <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>230</v>
-      </c>
-      <c r="L9" s="24">
-        <v>45615</v>
+        <v>222</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1634,10 +1814,10 @@
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>230</v>
-      </c>
-      <c r="L10" s="24">
-        <v>45616</v>
+        <v>222</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1672,10 +1852,10 @@
         <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>230</v>
-      </c>
-      <c r="L11" s="24">
-        <v>45617</v>
+        <v>222</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1710,10 +1890,10 @@
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>230</v>
-      </c>
-      <c r="L12" s="24">
-        <v>45618</v>
+        <v>222</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1748,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L13" s="24">
-        <v>45619</v>
+        <v>222</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1786,10 +1966,10 @@
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>230</v>
-      </c>
-      <c r="L14" s="24">
-        <v>45620</v>
+        <v>222</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1824,10 +2004,10 @@
         <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>230</v>
-      </c>
-      <c r="L15" s="24">
-        <v>45621</v>
+        <v>222</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1862,10 +2042,10 @@
         <v>18</v>
       </c>
       <c r="K16" t="s">
-        <v>230</v>
-      </c>
-      <c r="L16" s="24">
-        <v>45622</v>
+        <v>222</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1900,10 +2080,10 @@
         <v>12</v>
       </c>
       <c r="K17" t="s">
-        <v>230</v>
-      </c>
-      <c r="L17" s="24">
-        <v>45623</v>
+        <v>222</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1938,10 +2118,10 @@
         <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>230</v>
-      </c>
-      <c r="L18" s="24">
-        <v>45624</v>
+        <v>222</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1976,10 +2156,10 @@
         <v>5</v>
       </c>
       <c r="K19" t="s">
-        <v>230</v>
-      </c>
-      <c r="L19" s="24">
-        <v>45625</v>
+        <v>222</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2014,10 +2194,10 @@
         <v>22</v>
       </c>
       <c r="K20" t="s">
-        <v>230</v>
-      </c>
-      <c r="L20" s="24">
-        <v>45626</v>
+        <v>222</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2040,10 +2220,10 @@
         <v>8</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>21</v>
@@ -2052,10 +2232,10 @@
         <v>22</v>
       </c>
       <c r="K21" t="s">
-        <v>230</v>
-      </c>
-      <c r="L21" s="24">
-        <v>45627</v>
+        <v>222</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2078,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>19</v>
@@ -2090,10 +2270,10 @@
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>230</v>
-      </c>
-      <c r="L22" s="24">
-        <v>45628</v>
+        <v>222</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2116,10 +2296,10 @@
         <v>8</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>218</v>
+        <v>273</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>23</v>
@@ -2128,10 +2308,10 @@
         <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>230</v>
-      </c>
-      <c r="L23" s="24">
-        <v>45629</v>
+        <v>222</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2154,10 +2334,10 @@
         <v>8</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>220</v>
+        <v>83</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>23</v>
@@ -2166,10 +2346,10 @@
         <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>230</v>
-      </c>
-      <c r="L24" s="24">
-        <v>45630</v>
+        <v>222</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2192,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>15</v>
@@ -2204,10 +2384,10 @@
         <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>230</v>
-      </c>
-      <c r="L25" s="24">
-        <v>45631</v>
+        <v>222</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2230,10 +2410,10 @@
         <v>8</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>23</v>
@@ -2242,10 +2422,10 @@
         <v>24</v>
       </c>
       <c r="K26" t="s">
-        <v>230</v>
-      </c>
-      <c r="L26" s="24">
-        <v>45632</v>
+        <v>222</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2268,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>226</v>
+        <v>275</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>201</v>
@@ -2280,10 +2460,10 @@
         <v>202</v>
       </c>
       <c r="K27" t="s">
-        <v>230</v>
-      </c>
-      <c r="L27" s="24">
-        <v>45633</v>
+        <v>222</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2306,10 +2486,10 @@
         <v>8</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>228</v>
+        <v>276</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>30</v>
@@ -2318,10 +2498,10 @@
         <v>31</v>
       </c>
       <c r="K28" t="s">
-        <v>230</v>
-      </c>
-      <c r="L28" s="24">
-        <v>45634</v>
+        <v>222</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2344,7 +2524,7 @@
         <v>8</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>171</v>
+        <v>277</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>172</v>
@@ -2356,10 +2536,10 @@
         <v>22</v>
       </c>
       <c r="K29" t="s">
-        <v>230</v>
-      </c>
-      <c r="L29" s="24">
-        <v>45635</v>
+        <v>222</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2382,7 +2562,7 @@
         <v>8</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>176</v>
+        <v>278</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>177</v>
@@ -2394,10 +2574,10 @@
         <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>230</v>
-      </c>
-      <c r="L30" s="24">
-        <v>45636</v>
+        <v>222</v>
+      </c>
+      <c r="L30" s="24" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2420,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>181</v>
+        <v>291</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>182</v>
@@ -2432,10 +2612,10 @@
         <v>24</v>
       </c>
       <c r="K31" t="s">
-        <v>230</v>
-      </c>
-      <c r="L31" s="24">
-        <v>45637</v>
+        <v>222</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2458,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>154</v>
+        <v>276</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>155</v>
@@ -2470,10 +2650,10 @@
         <v>24</v>
       </c>
       <c r="K32" t="s">
-        <v>230</v>
-      </c>
-      <c r="L32" s="24">
-        <v>45638</v>
+        <v>222</v>
+      </c>
+      <c r="L32" s="24" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2496,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>189</v>
+        <v>274</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>190</v>
@@ -2508,10 +2688,10 @@
         <v>16</v>
       </c>
       <c r="K33" t="s">
-        <v>230</v>
-      </c>
-      <c r="L33" s="24">
-        <v>45639</v>
+        <v>222</v>
+      </c>
+      <c r="L33" s="24" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2534,7 +2714,7 @@
         <v>8</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>195</v>
@@ -2546,10 +2726,10 @@
         <v>24</v>
       </c>
       <c r="K34" t="s">
-        <v>230</v>
-      </c>
-      <c r="L34" s="24">
-        <v>45640</v>
+        <v>222</v>
+      </c>
+      <c r="L34" s="24" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2572,7 +2752,7 @@
         <v>8</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>199</v>
+        <v>289</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>200</v>
@@ -2584,10 +2764,10 @@
         <v>202</v>
       </c>
       <c r="K35" t="s">
-        <v>230</v>
-      </c>
-      <c r="L35" s="24">
-        <v>45641</v>
+        <v>222</v>
+      </c>
+      <c r="L35" s="24" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2610,7 +2790,7 @@
         <v>8</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>28</v>
+        <v>272</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>29</v>
@@ -2622,10 +2802,10 @@
         <v>31</v>
       </c>
       <c r="K36" t="s">
-        <v>230</v>
-      </c>
-      <c r="L36" s="24">
-        <v>45642</v>
+        <v>222</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2648,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>35</v>
+        <v>288</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>36</v>
@@ -2660,10 +2840,10 @@
         <v>24</v>
       </c>
       <c r="K37" t="s">
-        <v>230</v>
-      </c>
-      <c r="L37" s="24">
-        <v>45643</v>
+        <v>222</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2686,7 +2866,7 @@
         <v>8</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>40</v>
+        <v>287</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>41</v>
@@ -2698,10 +2878,10 @@
         <v>20</v>
       </c>
       <c r="K38" t="s">
-        <v>230</v>
-      </c>
-      <c r="L38" s="24">
-        <v>45644</v>
+        <v>222</v>
+      </c>
+      <c r="L38" s="24" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2724,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>45</v>
+        <v>275</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>46</v>
@@ -2736,10 +2916,10 @@
         <v>16</v>
       </c>
       <c r="K39" t="s">
-        <v>230</v>
-      </c>
-      <c r="L39" s="24">
-        <v>45645</v>
+        <v>222</v>
+      </c>
+      <c r="L39" s="24" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2762,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>51</v>
@@ -2774,10 +2954,10 @@
         <v>10</v>
       </c>
       <c r="K40" t="s">
-        <v>230</v>
-      </c>
-      <c r="L40" s="24">
-        <v>45646</v>
+        <v>222</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2800,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>55</v>
+        <v>285</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>56</v>
@@ -2812,10 +2992,10 @@
         <v>24</v>
       </c>
       <c r="K41" t="s">
-        <v>230</v>
-      </c>
-      <c r="L41" s="24">
-        <v>45647</v>
+        <v>222</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2838,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>60</v>
+        <v>284</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>61</v>
@@ -2850,10 +3030,10 @@
         <v>14</v>
       </c>
       <c r="K42" t="s">
-        <v>230</v>
-      </c>
-      <c r="L42" s="24">
-        <v>45648</v>
+        <v>222</v>
+      </c>
+      <c r="L42" s="24" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2876,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>65</v>
+        <v>283</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>66</v>
@@ -2888,10 +3068,10 @@
         <v>18</v>
       </c>
       <c r="K43" t="s">
-        <v>230</v>
-      </c>
-      <c r="L43" s="24">
-        <v>45649</v>
+        <v>222</v>
+      </c>
+      <c r="L43" s="24" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2914,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>70</v>
+        <v>282</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>71</v>
@@ -2926,10 +3106,10 @@
         <v>12</v>
       </c>
       <c r="K44" t="s">
-        <v>230</v>
-      </c>
-      <c r="L44" s="24">
-        <v>45650</v>
+        <v>222</v>
+      </c>
+      <c r="L44" s="24" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2952,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>75</v>
+        <v>281</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>76</v>
@@ -2964,10 +3144,10 @@
         <v>24</v>
       </c>
       <c r="K45" t="s">
-        <v>230</v>
-      </c>
-      <c r="L45" s="24">
-        <v>45651</v>
+        <v>222</v>
+      </c>
+      <c r="L45" s="24" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2990,7 +3170,7 @@
         <v>8</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>2</v>
+        <v>280</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>3</v>
@@ -3002,10 +3182,10 @@
         <v>5</v>
       </c>
       <c r="K46" t="s">
-        <v>230</v>
-      </c>
-      <c r="L46" s="24">
-        <v>45652</v>
+        <v>222</v>
+      </c>
+      <c r="L46" s="24" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3028,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>83</v>
+        <v>279</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>84</v>
@@ -3040,10 +3220,10 @@
         <v>22</v>
       </c>
       <c r="K47" t="s">
-        <v>230</v>
-      </c>
-      <c r="L47" s="24">
-        <v>45653</v>
+        <v>222</v>
+      </c>
+      <c r="L47" s="24" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>